<commit_message>
Limpieza de nombres de bienes de interés cultural
</commit_message>
<xml_diff>
--- a/documentos/Bienes_interes_cultural_cyl.xlsx
+++ b/documentos/Bienes_interes_cultural_cyl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectos\xaconews\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C31FF1-73D5-4742-A4F1-E2CBA25C94A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBF5EE8-3907-4587-A865-ED17BC31095B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -191,9 +191,6 @@
     <t>Crucero</t>
   </si>
   <si>
-    <t>Yacimiento de "Deobrigula"</t>
-  </si>
-  <si>
     <t>Hontanas</t>
   </si>
   <si>
@@ -239,9 +236,6 @@
     <t>Frómista</t>
   </si>
   <si>
-    <t>Canal de Castilla*</t>
-  </si>
-  <si>
     <t>Iglesia de San Martín</t>
   </si>
   <si>
@@ -320,9 +314,6 @@
     <t>Villamoros de Mansilla</t>
   </si>
   <si>
-    <t>Yacimiento arqueológico "Antigua Ciudad de Lancia"</t>
-  </si>
-  <si>
     <t>Villaverde de Sandoval</t>
   </si>
   <si>
@@ -461,15 +452,9 @@
     <t>El Casco Antiguo</t>
   </si>
   <si>
-    <t>Castillo de "El Temple"</t>
-  </si>
-  <si>
     <t>Cacabelos</t>
   </si>
   <si>
-    <t>Yacimiento arqueológico "La Edrada"</t>
-  </si>
-  <si>
     <t>Pieros</t>
   </si>
   <si>
@@ -509,13 +494,28 @@
     <t>Hórreo La Laguna</t>
   </si>
   <si>
-    <t>Central Térmica de la Minero Siderúrgica de Ponferrada - La fábrica de luz. Museo de la Energía</t>
-  </si>
-  <si>
     <t>Cueva Mayor - Portalón</t>
   </si>
   <si>
     <t>Cueva Mayor - Salón del Coro</t>
+  </si>
+  <si>
+    <t>Canal de Castilla</t>
+  </si>
+  <si>
+    <t>Yacimiento de Deobrigula</t>
+  </si>
+  <si>
+    <t>Yacimiento arqueológico Antigua Ciudad de Lancia</t>
+  </si>
+  <si>
+    <t>Castillo de El Temple</t>
+  </si>
+  <si>
+    <t>Yacimiento arqueológico La Edrada</t>
+  </si>
+  <si>
+    <t>Central Térmica de la Minero Siderúrgica de Ponferrada - La fábrica de luz - Museo de la Energía</t>
   </si>
 </sst>
 </file>
@@ -869,15 +869,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -989,7 +989,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1003,7 +1003,7 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1493,15 +1493,15 @@
         <v>15</v>
       </c>
       <c r="D44" t="s">
-        <v>51</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C45" t="s">
         <v>15</v>
@@ -1512,125 +1512,125 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" t="s">
         <v>52</v>
-      </c>
-      <c r="B46" t="s">
-        <v>52</v>
-      </c>
-      <c r="C46" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" t="s">
         <v>54</v>
-      </c>
-      <c r="B47" t="s">
-        <v>54</v>
-      </c>
-      <c r="C47" t="s">
-        <v>15</v>
-      </c>
-      <c r="D47" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C48" t="s">
         <v>15</v>
       </c>
       <c r="D48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C49" t="s">
         <v>15</v>
       </c>
       <c r="D49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C50" t="s">
         <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C51" t="s">
         <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C52" t="s">
         <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C53" t="s">
         <v>15</v>
       </c>
       <c r="D53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B54" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C54" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D54" t="s">
         <v>1</v>
@@ -1638,209 +1638,209 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D55" t="s">
-        <v>67</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56" t="s">
+        <v>79</v>
+      </c>
+      <c r="D56" t="s">
         <v>63</v>
-      </c>
-      <c r="B56" t="s">
-        <v>63</v>
-      </c>
-      <c r="C56" t="s">
-        <v>81</v>
-      </c>
-      <c r="D56" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C57" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D57" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B58" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D58" t="s">
-        <v>67</v>
+        <v>154</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59" t="s">
+        <v>79</v>
+      </c>
+      <c r="D59" t="s">
         <v>66</v>
-      </c>
-      <c r="B59" t="s">
-        <v>66</v>
-      </c>
-      <c r="C59" t="s">
-        <v>81</v>
-      </c>
-      <c r="D59" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C60" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D60" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C61" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D61" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B62" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C62" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D62" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B63" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C63" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D63" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B64" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C64" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D64" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65" t="s">
+        <v>72</v>
+      </c>
+      <c r="C65" t="s">
+        <v>79</v>
+      </c>
+      <c r="D65" t="s">
         <v>74</v>
-      </c>
-      <c r="B65" t="s">
-        <v>74</v>
-      </c>
-      <c r="C65" t="s">
-        <v>81</v>
-      </c>
-      <c r="D65" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B66" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C66" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D66" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>77</v>
+      </c>
+      <c r="B67" t="s">
+        <v>77</v>
+      </c>
+      <c r="C67" t="s">
         <v>79</v>
       </c>
-      <c r="B67" t="s">
-        <v>79</v>
-      </c>
-      <c r="C67" t="s">
-        <v>81</v>
-      </c>
       <c r="D67" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B68" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C68" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D68" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B69" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C69" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D69" t="s">
         <v>19</v>
@@ -1848,195 +1848,195 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B70" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C70" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D70" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B71" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C71" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D71" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B72" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C72" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D72" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B73" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C73" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D73" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>82</v>
+      </c>
+      <c r="B74" t="s">
+        <v>82</v>
+      </c>
+      <c r="C74" t="s">
+        <v>94</v>
+      </c>
+      <c r="D74" t="s">
         <v>84</v>
-      </c>
-      <c r="B74" t="s">
-        <v>84</v>
-      </c>
-      <c r="C74" t="s">
-        <v>97</v>
-      </c>
-      <c r="D74" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B75" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C75" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D75" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B76" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C76" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D76" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B77" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C77" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D77" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B78" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C78" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D78" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
+        <v>87</v>
+      </c>
+      <c r="B79" t="s">
+        <v>87</v>
+      </c>
+      <c r="C79" t="s">
+        <v>94</v>
+      </c>
+      <c r="D79" t="s">
         <v>89</v>
-      </c>
-      <c r="B79" t="s">
-        <v>89</v>
-      </c>
-      <c r="C79" t="s">
-        <v>97</v>
-      </c>
-      <c r="D79" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B80" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C80" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D80" t="s">
-        <v>94</v>
+        <v>156</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>90</v>
+      </c>
+      <c r="B81" t="s">
         <v>92</v>
       </c>
-      <c r="B81" t="s">
-        <v>95</v>
-      </c>
       <c r="C81" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D81" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B82" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C82" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D82" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B83" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C83" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D83" t="s">
         <v>17</v>
@@ -2044,13 +2044,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B84" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C84" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D84" t="s">
         <v>18</v>
@@ -2058,97 +2058,97 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B85" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C85" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D85" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
+        <v>94</v>
+      </c>
+      <c r="B86" t="s">
+        <v>94</v>
+      </c>
+      <c r="C86" t="s">
+        <v>94</v>
+      </c>
+      <c r="D86" t="s">
         <v>97</v>
-      </c>
-      <c r="B86" t="s">
-        <v>97</v>
-      </c>
-      <c r="C86" t="s">
-        <v>97</v>
-      </c>
-      <c r="D86" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B87" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C87" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D87" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B88" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C88" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D88" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B89" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C89" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D89" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B90" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C90" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D90" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B91" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C91" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D91" t="s">
         <v>37</v>
@@ -2156,195 +2156,195 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B92" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C92" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D92" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B93" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C93" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D93" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C94" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D94" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C95" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D95" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C96" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D96" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B97" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C97" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D97" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B98" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C98" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D98" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B99" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C99" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D99" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B100" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C100" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D100" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B101" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C101" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D101" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B102" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C102" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D102" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B103" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C103" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D103" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B104" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C104" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D104" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B105" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C105" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D105" t="s">
         <v>50</v>
@@ -2352,139 +2352,139 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B106" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C106" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D106" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B107" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C107" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D107" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
+        <v>118</v>
+      </c>
+      <c r="B108" t="s">
+        <v>118</v>
+      </c>
+      <c r="C108" t="s">
+        <v>94</v>
+      </c>
+      <c r="D108" t="s">
         <v>121</v>
-      </c>
-      <c r="B108" t="s">
-        <v>121</v>
-      </c>
-      <c r="C108" t="s">
-        <v>97</v>
-      </c>
-      <c r="D108" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B109" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C109" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D109" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B110" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C110" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D110" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B111" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C111" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D111" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B112" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C112" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D112" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B113" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C113" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D113" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
+        <v>126</v>
+      </c>
+      <c r="B114" t="s">
+        <v>126</v>
+      </c>
+      <c r="C114" t="s">
+        <v>94</v>
+      </c>
+      <c r="D114" t="s">
         <v>129</v>
-      </c>
-      <c r="B114" t="s">
-        <v>129</v>
-      </c>
-      <c r="C114" t="s">
-        <v>97</v>
-      </c>
-      <c r="D114" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B115" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C115" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D115" t="s">
         <v>37</v>
@@ -2492,139 +2492,139 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B116" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C116" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D116" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B117" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C117" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D117" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B118" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C118" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D118" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B119" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C119" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D119" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B120" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C120" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D120" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B121" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C121" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D121" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B122" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C122" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D122" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B123" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C123" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D123" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B124" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C124" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D124" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B125" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C125" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D125" t="s">
         <v>19</v>
@@ -2632,156 +2632,156 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B126" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C126" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D126" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B127" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C127" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D127" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B128" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C128" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D128" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
+        <v>141</v>
+      </c>
+      <c r="B129" t="s">
+        <v>141</v>
+      </c>
+      <c r="C129" t="s">
+        <v>94</v>
+      </c>
+      <c r="D129" t="s">
         <v>146</v>
-      </c>
-      <c r="B129" t="s">
-        <v>146</v>
-      </c>
-      <c r="C129" t="s">
-        <v>97</v>
-      </c>
-      <c r="D129" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B130" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C130" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D130" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B131" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C131" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D131" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B132" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C132" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D132" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B133" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C133" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D133" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B134" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C134" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D134" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B135" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C135" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D135" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B136" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C136" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D136" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios definitivos formato Bienes culturales CyL
</commit_message>
<xml_diff>
--- a/documentos/Bienes_interes_cultural_cyl.xlsx
+++ b/documentos/Bienes_interes_cultural_cyl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectos\xaconews\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBF5EE8-3907-4587-A865-ED17BC31095B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CD0981-395B-480E-BF0F-AAD5C952CFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -125,9 +125,6 @@
     <t>Casa del Cordón</t>
   </si>
   <si>
-    <t>Casa de Miranda, Museo de Burgos</t>
-  </si>
-  <si>
     <t>Monasterio de San Juan</t>
   </si>
   <si>
@@ -516,6 +513,9 @@
   </si>
   <si>
     <t>Central Térmica de la Minero Siderúrgica de Ponferrada - La fábrica de luz - Museo de la Energía</t>
+  </si>
+  <si>
+    <t>Casa de Miranda Museo de Burgos</t>
   </si>
 </sst>
 </file>
@@ -869,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="D137" sqref="D137"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -989,7 +989,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1003,7 +1003,7 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1199,7 +1199,7 @@
         <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1213,7 +1213,7 @@
         <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1227,7 +1227,7 @@
         <v>15</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1241,7 +1241,7 @@
         <v>15</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1255,7 +1255,7 @@
         <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1269,7 +1269,7 @@
         <v>15</v>
       </c>
       <c r="D28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1283,7 +1283,7 @@
         <v>15</v>
       </c>
       <c r="D29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1297,7 +1297,7 @@
         <v>15</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1311,7 +1311,7 @@
         <v>15</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1325,7 +1325,7 @@
         <v>15</v>
       </c>
       <c r="D32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1339,7 +1339,7 @@
         <v>15</v>
       </c>
       <c r="D33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1353,7 +1353,7 @@
         <v>15</v>
       </c>
       <c r="D34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1367,7 +1367,7 @@
         <v>15</v>
       </c>
       <c r="D35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1381,7 +1381,7 @@
         <v>15</v>
       </c>
       <c r="D36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1395,7 +1395,7 @@
         <v>15</v>
       </c>
       <c r="D37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1409,7 +1409,7 @@
         <v>15</v>
       </c>
       <c r="D38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1423,7 +1423,7 @@
         <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1437,7 +1437,7 @@
         <v>15</v>
       </c>
       <c r="D40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1451,7 +1451,7 @@
         <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1465,172 +1465,172 @@
         <v>15</v>
       </c>
       <c r="D42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" t="s">
         <v>49</v>
-      </c>
-      <c r="B43" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43" t="s">
-        <v>15</v>
-      </c>
-      <c r="D43" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C44" t="s">
         <v>15</v>
       </c>
       <c r="D44" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C45" t="s">
         <v>15</v>
       </c>
       <c r="D45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" t="s">
         <v>51</v>
-      </c>
-      <c r="B46" t="s">
-        <v>51</v>
-      </c>
-      <c r="C46" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" t="s">
         <v>53</v>
-      </c>
-      <c r="B47" t="s">
-        <v>53</v>
-      </c>
-      <c r="C47" t="s">
-        <v>15</v>
-      </c>
-      <c r="D47" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C48" t="s">
         <v>15</v>
       </c>
       <c r="D48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
         <v>15</v>
       </c>
       <c r="D49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C50" t="s">
         <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C51" t="s">
         <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C52" t="s">
         <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C53" t="s">
         <v>15</v>
       </c>
       <c r="D53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D54" t="s">
         <v>1</v>
@@ -1638,209 +1638,209 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D55" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" t="s">
+        <v>78</v>
+      </c>
+      <c r="D56" t="s">
         <v>62</v>
-      </c>
-      <c r="B56" t="s">
-        <v>62</v>
-      </c>
-      <c r="C56" t="s">
-        <v>79</v>
-      </c>
-      <c r="D56" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D57" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D58" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" t="s">
+        <v>78</v>
+      </c>
+      <c r="D59" t="s">
         <v>65</v>
-      </c>
-      <c r="B59" t="s">
-        <v>65</v>
-      </c>
-      <c r="C59" t="s">
-        <v>79</v>
-      </c>
-      <c r="D59" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C60" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D60" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D61" t="s">
         <v>68</v>
-      </c>
-      <c r="B61" t="s">
-        <v>68</v>
-      </c>
-      <c r="C61" t="s">
-        <v>79</v>
-      </c>
-      <c r="D61" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B62" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D63" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" t="s">
+        <v>78</v>
+      </c>
+      <c r="D64" t="s">
         <v>72</v>
-      </c>
-      <c r="B64" t="s">
-        <v>72</v>
-      </c>
-      <c r="C64" t="s">
-        <v>79</v>
-      </c>
-      <c r="D64" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B65" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C65" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>74</v>
+      </c>
+      <c r="B66" t="s">
+        <v>74</v>
+      </c>
+      <c r="C66" t="s">
+        <v>78</v>
+      </c>
+      <c r="D66" t="s">
         <v>75</v>
-      </c>
-      <c r="B66" t="s">
-        <v>75</v>
-      </c>
-      <c r="C66" t="s">
-        <v>79</v>
-      </c>
-      <c r="D66" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>76</v>
+      </c>
+      <c r="B67" t="s">
+        <v>76</v>
+      </c>
+      <c r="C67" t="s">
+        <v>78</v>
+      </c>
+      <c r="D67" t="s">
         <v>77</v>
-      </c>
-      <c r="B67" t="s">
-        <v>77</v>
-      </c>
-      <c r="C67" t="s">
-        <v>79</v>
-      </c>
-      <c r="D67" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C68" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D68" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B69" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D69" t="s">
         <v>19</v>
@@ -1848,195 +1848,195 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>79</v>
+      </c>
+      <c r="B70" t="s">
+        <v>79</v>
+      </c>
+      <c r="C70" t="s">
+        <v>93</v>
+      </c>
+      <c r="D70" t="s">
         <v>80</v>
-      </c>
-      <c r="B70" t="s">
-        <v>80</v>
-      </c>
-      <c r="C70" t="s">
-        <v>94</v>
-      </c>
-      <c r="D70" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C71" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D71" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B72" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C72" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D72" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>81</v>
+      </c>
+      <c r="B73" t="s">
+        <v>81</v>
+      </c>
+      <c r="C73" t="s">
+        <v>93</v>
+      </c>
+      <c r="D73" t="s">
         <v>82</v>
-      </c>
-      <c r="B73" t="s">
-        <v>82</v>
-      </c>
-      <c r="C73" t="s">
-        <v>94</v>
-      </c>
-      <c r="D73" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B74" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C74" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D74" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B75" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C75" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D75" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B76" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C76" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D76" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>86</v>
+      </c>
+      <c r="B77" t="s">
+        <v>86</v>
+      </c>
+      <c r="C77" t="s">
+        <v>93</v>
+      </c>
+      <c r="D77" t="s">
         <v>87</v>
-      </c>
-      <c r="B77" t="s">
-        <v>87</v>
-      </c>
-      <c r="C77" t="s">
-        <v>94</v>
-      </c>
-      <c r="D77" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
+        <v>86</v>
+      </c>
+      <c r="B78" t="s">
+        <v>86</v>
+      </c>
+      <c r="C78" t="s">
+        <v>93</v>
+      </c>
+      <c r="D78" t="s">
         <v>87</v>
-      </c>
-      <c r="B78" t="s">
-        <v>87</v>
-      </c>
-      <c r="C78" t="s">
-        <v>94</v>
-      </c>
-      <c r="D78" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C79" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D79" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
+        <v>89</v>
+      </c>
+      <c r="B80" t="s">
         <v>90</v>
       </c>
-      <c r="B80" t="s">
-        <v>91</v>
-      </c>
       <c r="C80" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D80" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B81" t="s">
+        <v>91</v>
+      </c>
+      <c r="C81" t="s">
+        <v>93</v>
+      </c>
+      <c r="D81" t="s">
         <v>92</v>
-      </c>
-      <c r="C81" t="s">
-        <v>94</v>
-      </c>
-      <c r="D81" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
+        <v>93</v>
+      </c>
+      <c r="B82" t="s">
+        <v>93</v>
+      </c>
+      <c r="C82" t="s">
+        <v>93</v>
+      </c>
+      <c r="D82" t="s">
         <v>94</v>
-      </c>
-      <c r="B82" t="s">
-        <v>94</v>
-      </c>
-      <c r="C82" t="s">
-        <v>94</v>
-      </c>
-      <c r="D82" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B83" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C83" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D83" t="s">
         <v>17</v>
@@ -2044,13 +2044,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B84" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C84" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D84" t="s">
         <v>18</v>
@@ -2058,573 +2058,573 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B85" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C85" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D85" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B86" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C86" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D86" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B87" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C87" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D87" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B88" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C88" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D88" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D89" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B90" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C90" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D90" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C91" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D91" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B92" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C92" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D92" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C93" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D93" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C94" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D94" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C95" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D95" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B96" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C96" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D96" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B97" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C97" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D97" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B98" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C98" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D98" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B99" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C99" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D99" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B100" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C100" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D100" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B101" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C101" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D101" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B102" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C102" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D102" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B103" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C103" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D103" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B104" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C104" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D104" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
+        <v>114</v>
+      </c>
+      <c r="B105" t="s">
         <v>115</v>
       </c>
-      <c r="B105" t="s">
-        <v>116</v>
-      </c>
       <c r="C105" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D105" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B106" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C106" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D106" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
+        <v>117</v>
+      </c>
+      <c r="B107" t="s">
         <v>118</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
+        <v>93</v>
+      </c>
+      <c r="D107" t="s">
         <v>119</v>
-      </c>
-      <c r="C107" t="s">
-        <v>94</v>
-      </c>
-      <c r="D107" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B108" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C108" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D108" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
+        <v>121</v>
+      </c>
+      <c r="B109" t="s">
+        <v>121</v>
+      </c>
+      <c r="C109" t="s">
+        <v>93</v>
+      </c>
+      <c r="D109" t="s">
         <v>122</v>
-      </c>
-      <c r="B109" t="s">
-        <v>122</v>
-      </c>
-      <c r="C109" t="s">
-        <v>94</v>
-      </c>
-      <c r="D109" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
+        <v>123</v>
+      </c>
+      <c r="B110" t="s">
+        <v>123</v>
+      </c>
+      <c r="C110" t="s">
+        <v>93</v>
+      </c>
+      <c r="D110" t="s">
         <v>124</v>
-      </c>
-      <c r="B110" t="s">
-        <v>124</v>
-      </c>
-      <c r="C110" t="s">
-        <v>94</v>
-      </c>
-      <c r="D110" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
+        <v>125</v>
+      </c>
+      <c r="B111" t="s">
+        <v>125</v>
+      </c>
+      <c r="C111" t="s">
+        <v>93</v>
+      </c>
+      <c r="D111" t="s">
         <v>126</v>
-      </c>
-      <c r="B111" t="s">
-        <v>126</v>
-      </c>
-      <c r="C111" t="s">
-        <v>94</v>
-      </c>
-      <c r="D111" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B112" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C112" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D112" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B113" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C113" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D113" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B114" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C114" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D114" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B115" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C115" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D115" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B116" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C116" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D116" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B117" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C117" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D117" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
+        <v>131</v>
+      </c>
+      <c r="B118" t="s">
         <v>132</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" t="s">
+        <v>93</v>
+      </c>
+      <c r="D118" t="s">
         <v>133</v>
-      </c>
-      <c r="C118" t="s">
-        <v>94</v>
-      </c>
-      <c r="D118" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B119" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C119" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D119" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
+        <v>135</v>
+      </c>
+      <c r="B120" t="s">
+        <v>135</v>
+      </c>
+      <c r="C120" t="s">
+        <v>93</v>
+      </c>
+      <c r="D120" t="s">
         <v>136</v>
-      </c>
-      <c r="B120" t="s">
-        <v>136</v>
-      </c>
-      <c r="C120" t="s">
-        <v>94</v>
-      </c>
-      <c r="D120" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B121" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C121" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D121" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B122" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C122" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D122" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
+        <v>137</v>
+      </c>
+      <c r="B123" t="s">
         <v>138</v>
       </c>
-      <c r="B123" t="s">
+      <c r="C123" t="s">
+        <v>93</v>
+      </c>
+      <c r="D123" t="s">
         <v>139</v>
-      </c>
-      <c r="C123" t="s">
-        <v>94</v>
-      </c>
-      <c r="D123" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
+        <v>140</v>
+      </c>
+      <c r="B124" t="s">
+        <v>140</v>
+      </c>
+      <c r="C124" t="s">
+        <v>93</v>
+      </c>
+      <c r="D124" t="s">
         <v>141</v>
-      </c>
-      <c r="B124" t="s">
-        <v>141</v>
-      </c>
-      <c r="C124" t="s">
-        <v>94</v>
-      </c>
-      <c r="D124" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B125" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C125" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D125" t="s">
         <v>19</v>
@@ -2632,156 +2632,156 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B126" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C126" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D126" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B127" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C127" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D127" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B128" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C128" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D128" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B129" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C129" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D129" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B130" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C130" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D130" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
+        <v>146</v>
+      </c>
+      <c r="B131" t="s">
+        <v>146</v>
+      </c>
+      <c r="C131" t="s">
+        <v>93</v>
+      </c>
+      <c r="D131" t="s">
         <v>147</v>
-      </c>
-      <c r="B131" t="s">
-        <v>147</v>
-      </c>
-      <c r="C131" t="s">
-        <v>94</v>
-      </c>
-      <c r="D131" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B132" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C132" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D132" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B133" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C133" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D133" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B134" t="s">
+        <v>149</v>
+      </c>
+      <c r="C134" t="s">
+        <v>93</v>
+      </c>
+      <c r="D134" t="s">
         <v>150</v>
-      </c>
-      <c r="C134" t="s">
-        <v>94</v>
-      </c>
-      <c r="D134" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B135" t="s">
+        <v>149</v>
+      </c>
+      <c r="C135" t="s">
+        <v>93</v>
+      </c>
+      <c r="D135" t="s">
         <v>150</v>
-      </c>
-      <c r="C135" t="s">
-        <v>94</v>
-      </c>
-      <c r="D135" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C136" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D136" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>